<commit_message>
Update smoke test file
</commit_message>
<xml_diff>
--- a/documents/Test Case/Smoke test - case for automation.xlsx
+++ b/documents/Test Case/Smoke test - case for automation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -211,6 +211,12 @@
   <si>
     <t>TCSL_009/
 TCSL_016</t>
+  </si>
+  <si>
+    <t>User should be routed to the search products page</t>
+  </si>
+  <si>
+    <t>Check that the user has landed on the my account page</t>
   </si>
 </sst>
 </file>
@@ -401,20 +407,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,14 +707,14 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="22" customWidth="1"/>
     <col min="3" max="3" width="92.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" style="16" customWidth="1"/>
@@ -737,13 +743,13 @@
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
@@ -753,9 +759,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="22"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="20"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
@@ -765,9 +771,9 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="22"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
@@ -777,9 +783,9 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="22"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="20"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="14" t="s">
         <v>16</v>
       </c>
@@ -789,27 +795,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="22"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="20"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="14" t="s">
         <v>4</v>
       </c>
@@ -819,9 +825,9 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="22"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="20"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
@@ -831,9 +837,9 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="22"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="14" t="s">
         <v>14</v>
       </c>
@@ -843,9 +849,9 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="22"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
       </c>
@@ -855,9 +861,9 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="22"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="20"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="14" t="s">
         <v>17</v>
       </c>
@@ -867,9 +873,9 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="22"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="20"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="14" t="s">
         <v>25</v>
       </c>
@@ -879,9 +885,9 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="22"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="14" t="s">
         <v>26</v>
       </c>
@@ -891,9 +897,9 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="22"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="14" t="s">
         <v>28</v>
       </c>
@@ -911,7 +917,7 @@
       <c r="C15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="14" t="s">
         <v>4</v>
       </c>
@@ -921,9 +927,9 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="22"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="14" t="s">
         <v>7</v>
       </c>
@@ -933,9 +939,9 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="22"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="14" t="s">
         <v>14</v>
       </c>
@@ -945,9 +951,9 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="22"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
@@ -957,9 +963,9 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="22"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="20"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="14" t="s">
         <v>17</v>
       </c>
@@ -969,9 +975,9 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="22"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="14" t="s">
         <v>25</v>
       </c>
@@ -981,9 +987,9 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="22"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="14" t="s">
         <v>26</v>
       </c>
@@ -993,21 +999,21 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="22"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="20"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="22"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="14">
         <v>9</v>
       </c>
@@ -1017,9 +1023,9 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="22"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="14">
         <v>10</v>
       </c>
@@ -1031,13 +1037,13 @@
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="20"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="14" t="s">
         <v>4</v>
       </c>
@@ -1047,9 +1053,9 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="22"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="14" t="s">
         <v>7</v>
       </c>
@@ -1059,9 +1065,9 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="22"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="14" t="s">
         <v>14</v>
       </c>
@@ -1071,9 +1077,9 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="22"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="14" t="s">
         <v>16</v>
       </c>
@@ -1083,9 +1089,9 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="22"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="14" t="s">
         <v>17</v>
       </c>
@@ -1097,13 +1103,13 @@
       <c r="A30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="14" t="s">
         <v>4</v>
       </c>
@@ -1113,9 +1119,9 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="22"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="20"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="14" t="s">
         <v>7</v>
       </c>
@@ -1125,9 +1131,9 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="22"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="20"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="14" t="s">
         <v>14</v>
       </c>
@@ -1137,9 +1143,9 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="22"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="20"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="14" t="s">
         <v>16</v>
       </c>
@@ -1149,9 +1155,9 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="22"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="14" t="s">
         <v>46</v>
       </c>
@@ -1161,9 +1167,9 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="22"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="20"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="14" t="s">
         <v>25</v>
       </c>
@@ -1173,9 +1179,9 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="22"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="14" t="s">
         <v>26</v>
       </c>
@@ -1185,9 +1191,9 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="22"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="14" t="s">
         <v>28</v>
       </c>
@@ -1197,9 +1203,9 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="22"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="20"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="14" t="s">
         <v>35</v>
       </c>
@@ -1209,9 +1215,9 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="22"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="20"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="14" t="s">
         <v>48</v>
       </c>
@@ -1221,9 +1227,9 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="22"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="20"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="14" t="s">
         <v>49</v>
       </c>
@@ -1233,9 +1239,9 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="22"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="20"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="14" t="s">
         <v>51</v>
       </c>
@@ -1245,9 +1251,9 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="22"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="20"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="14" t="s">
         <v>52</v>
       </c>
@@ -1257,9 +1263,9 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="22"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="23"/>
       <c r="E43" s="14" t="s">
         <v>54</v>
       </c>
@@ -1269,9 +1275,9 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="22"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="9"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="14" t="s">
         <v>55</v>
       </c>
@@ -1281,9 +1287,9 @@
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
-      <c r="B45" s="23"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="12"/>
-      <c r="D45" s="21"/>
+      <c r="D45" s="24"/>
       <c r="E45" s="15" t="s">
         <v>58</v>
       </c>

</xml_diff>